<commit_message>
bibliotecas e inicia testes
</commit_message>
<xml_diff>
--- a/src/info/aquis_censo_matricula_cols.xlsx
+++ b/src/info/aquis_censo_matricula_cols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.forli\PycharmProjects\curso-ciencia-dados\src\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8121FA9E-F92B-4862-8059-5AAB7880D26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72AC956-3FE5-4158-938F-C4A21E6A243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48C7DDBA-442F-4222-8A07-8EDC411B5A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48C7DDBA-442F-4222-8A07-8EDC411B5A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="dtype" sheetId="14" r:id="rId1"/>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="M109" sqref="M109"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2552,7 @@
         <v>125</v>
       </c>
       <c r="C118" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -11974,7 +11974,7 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B39"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>